<commit_message>
Se elimina el recuperación de vencimientos del Informe Completo de Nevasa
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20250210/20250210_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20250210/20250210_informe_completo_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>compra/venta/vencimiento</t>
+          <t>compra/venta</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -625,27 +625,27 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>66344960</v>
+        <v>20090783.801</v>
       </c>
       <c r="F5" t="n">
-        <v>66344960</v>
+        <v>19725963</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>LTM</t>
+          <t>INDISA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>VCTO</t>
+          <t>VENTA</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>VENCIMIENTO</t>
+          <t>SIMULTANEA</t>
         </is>
       </c>
     </row>
@@ -662,30 +662,30 @@
         <v>45698</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.4117</v>
       </c>
       <c r="E6" t="n">
-        <v>216541946</v>
+        <v>1400000000</v>
       </c>
       <c r="F6" t="n">
-        <v>216541946</v>
+        <v>1398081440</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>LAS CONDES</t>
+          <t>BNPDBC200225</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>VCTO</t>
+          <t>COMPRA</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>VENCIMIENTO</t>
+          <t>RENTA VARIABLE</t>
         </is>
       </c>
     </row>
@@ -702,30 +702,30 @@
         <v>45698</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>16871</v>
       </c>
       <c r="E7" t="n">
-        <v>20090783.801</v>
+        <v>14</v>
       </c>
       <c r="F7" t="n">
-        <v>19725963</v>
+        <v>236194</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>INDISA</t>
+          <t>CFINHRFLA</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>VENTA</t>
+          <t>COMPRA</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>SIMULTANEA</t>
+          <t>RENTA VARIABLE</t>
         </is>
       </c>
     </row>
@@ -742,20 +742,20 @@
         <v>45698</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4117</v>
+        <v>16871.4</v>
       </c>
       <c r="E8" t="n">
-        <v>1400000000</v>
+        <v>3790</v>
       </c>
       <c r="F8" t="n">
-        <v>1398081440</v>
+        <v>63942604</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>BNPDBC200225</t>
+          <t>CFINHRFLA</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -782,20 +782,20 @@
         <v>45698</v>
       </c>
       <c r="D9" t="n">
-        <v>16871</v>
+        <v>16319.89</v>
       </c>
       <c r="E9" t="n">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="F9" t="n">
-        <v>236194</v>
+        <v>995513</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>CFINHRFLA</t>
+          <t>CFINHRFLB</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -804,86 +804,6 @@
         </is>
       </c>
       <c r="J9" t="inlineStr">
-        <is>
-          <t>RENTA VARIABLE</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>FONDO DE INVERSION NEVASA AHORRO</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>45698</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>45698</v>
-      </c>
-      <c r="D10" t="n">
-        <v>16871.4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3790</v>
-      </c>
-      <c r="F10" t="n">
-        <v>63942604</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>CFINHRFLA</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>COMPRA</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>RENTA VARIABLE</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FONDO DE INVERSION NEVASA AHORRO</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>45698</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>45698</v>
-      </c>
-      <c r="D11" t="n">
-        <v>16319.89</v>
-      </c>
-      <c r="E11" t="n">
-        <v>61</v>
-      </c>
-      <c r="F11" t="n">
-        <v>995513</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>CFINHRFLB</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>COMPRA</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
         <is>
           <t>RENTA VARIABLE</t>
         </is>

</xml_diff>